<commit_message>
added coverage percentage to excel
</commit_message>
<xml_diff>
--- a/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5162CBD-E3FC-4E55-8884-54931504A2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E84E35-1107-445E-AB27-5DD9A8622698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -1417,11 +1417,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1453,6 +1451,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1462,6 +1463,54 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1471,53 +1520,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1525,44 +1544,89 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1579,9 +1643,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1630,69 +1691,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2140,15 +2140,15 @@
   <sheetData>
     <row r="1" spans="2:16">
       <c r="B1" s="11"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="2:16">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2166,21 +2166,21 @@
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26" t="s">
+      <c r="N6" s="25"/>
+      <c r="O6" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="P6" s="25" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2189,13 +2189,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="25">
         <v>237</v>
       </c>
     </row>
@@ -2204,13 +2204,13 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="26" t="s">
+      <c r="O8" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="25">
         <v>237</v>
       </c>
     </row>
@@ -2221,11 +2221,11 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="26" t="s">
+      <c r="N9" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" t="s">
@@ -2236,7 +2236,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="1"/>
@@ -2249,7 +2249,7 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2275,7 +2275,7 @@
   </sheetPr>
   <dimension ref="B1:X24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -2288,28 +2288,28 @@
   <sheetData>
     <row r="1" spans="2:24">
       <c r="B1" s="11"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="3" spans="2:24">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="5" spans="2:24">
       <c r="R5" t="s">
@@ -2332,55 +2332,55 @@
       </c>
     </row>
     <row r="6" spans="2:24">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="I6" s="44" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="I6" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="Q6" s="44" t="s">
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="Q6" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
     </row>
     <row r="8" spans="2:24">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
       <c r="I8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="51" t="s">
+      <c r="Q8" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="33">
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:24">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="50" t="s">
@@ -2388,20 +2388,20 @@
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="I9" s="37"/>
-      <c r="Q9" s="51" t="s">
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="I9" s="35"/>
+      <c r="Q9" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="33" t="s">
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="31" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:24">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="50" t="s">
@@ -2409,30 +2409,30 @@
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="I10" s="56" t="s">
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="I10" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="58"/>
-      <c r="Q10" s="51" t="s">
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="53"/>
+      <c r="Q10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="51" t="s">
+      <c r="R10" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="51"/>
-      <c r="T10" s="33" t="s">
+      <c r="S10" s="60"/>
+      <c r="T10" s="31" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:24">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="50" t="s">
@@ -2440,18 +2440,18 @@
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="61"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="56"/>
     </row>
     <row r="12" spans="2:24">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="50" t="s">
@@ -2459,18 +2459,18 @@
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="61"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="56"/>
     </row>
     <row r="13" spans="2:24">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="50" t="s">
@@ -2478,24 +2478,24 @@
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="61"/>
-      <c r="Q13" s="44" t="s">
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="56"/>
+      <c r="Q13" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
     </row>
     <row r="14" spans="2:24">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="32" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="50" t="s">
@@ -2503,163 +2503,171 @@
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="61"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="56"/>
     </row>
     <row r="15" spans="2:24">
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="61"/>
-      <c r="Q15" s="31" t="s">
+      <c r="I15" s="54"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="56"/>
+      <c r="Q15" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="65" t="s">
+      <c r="R15" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="65"/>
-      <c r="T15" s="65"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
     </row>
     <row r="16" spans="2:24">
-      <c r="I16" s="59"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="61"/>
-      <c r="Q16" s="34" t="s">
+      <c r="I16" s="54"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="56"/>
+      <c r="Q16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="R16" s="47" t="s">
+      <c r="R16" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="S16" s="48"/>
-      <c r="T16" s="49"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="64"/>
       <c r="V16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="9:20">
-      <c r="I17" s="59"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="61"/>
-      <c r="Q17" s="34" t="s">
+      <c r="I17" s="54"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="56"/>
+      <c r="Q17" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="R17" s="47" t="s">
+      <c r="R17" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="S17" s="48"/>
-      <c r="T17" s="49"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="64"/>
     </row>
     <row r="18" spans="9:20">
-      <c r="I18" s="59"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="61"/>
-      <c r="Q18" s="34" t="s">
+      <c r="I18" s="54"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="56"/>
+      <c r="Q18" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R18" s="47" t="s">
+      <c r="R18" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="S18" s="48"/>
-      <c r="T18" s="49"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="64"/>
     </row>
     <row r="19" spans="9:20">
-      <c r="I19" s="59"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="61"/>
-      <c r="Q19" s="34" t="s">
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="56"/>
+      <c r="Q19" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="R19" s="47" t="s">
+      <c r="R19" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="S19" s="48"/>
-      <c r="T19" s="49"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="64"/>
     </row>
     <row r="20" spans="9:20">
-      <c r="I20" s="59"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="61"/>
-      <c r="Q20" s="34" t="s">
+      <c r="I20" s="54"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="56"/>
+      <c r="Q20" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="R20" s="52" t="s">
+      <c r="R20" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
     </row>
     <row r="21" spans="9:20">
-      <c r="I21" s="59"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="61"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="52"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="56"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
     </row>
     <row r="22" spans="9:20">
-      <c r="I22" s="59"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="61"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="56"/>
     </row>
     <row r="23" spans="9:20">
-      <c r="I23" s="59"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="56"/>
     </row>
     <row r="24" spans="9:20">
-      <c r="I24" s="62"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="64"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2676,14 +2684,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2729,168 +2729,168 @@
     <row r="1" spans="2:26">
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="3" spans="2:26">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="5" spans="2:26">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="2:26" ht="15.75">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="75" t="s">
+      <c r="D6" s="76"/>
+      <c r="E6" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="80"/>
-      <c r="S6" s="80"/>
-      <c r="T6" s="80"/>
-      <c r="U6" s="80"/>
-      <c r="V6" s="80"/>
-      <c r="W6" s="80"/>
-      <c r="X6" s="80"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="80"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="67"/>
+      <c r="Z6" s="67"/>
     </row>
     <row r="7" spans="2:26" ht="15.75">
-      <c r="B7" s="80"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="68" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="69" t="s">
+      <c r="G7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="70" t="s">
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="P7" s="70"/>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="70"/>
-      <c r="S7" s="70"/>
-      <c r="T7" s="77" t="s">
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="77"/>
-      <c r="V7" s="77"/>
-      <c r="W7" s="77"/>
-      <c r="X7" s="77"/>
-      <c r="Y7" s="77"/>
-      <c r="Z7" s="77"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="70"/>
+      <c r="X7" s="70"/>
+      <c r="Y7" s="70"/>
+      <c r="Z7" s="70"/>
     </row>
     <row r="8" spans="2:26" ht="15.6" customHeight="1">
-      <c r="B8" s="80"/>
-      <c r="C8" s="75" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="D8" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="68"/>
-      <c r="G8" s="69" t="s">
+      <c r="F8" s="79"/>
+      <c r="G8" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69" t="s">
+      <c r="H8" s="73"/>
+      <c r="I8" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69" t="s">
+      <c r="J8" s="73"/>
+      <c r="K8" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69" t="s">
+      <c r="L8" s="73"/>
+      <c r="M8" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="N8" s="69"/>
-      <c r="O8" s="70" t="s">
+      <c r="N8" s="73"/>
+      <c r="O8" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="Q8" s="70" t="s">
+      <c r="Q8" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="R8" s="70" t="s">
+      <c r="R8" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="S8" s="70" t="s">
+      <c r="S8" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="T8" s="77">
+      <c r="T8" s="70">
         <v>0</v>
       </c>
-      <c r="U8" s="77">
+      <c r="U8" s="70">
         <v>1</v>
       </c>
-      <c r="V8" s="77">
+      <c r="V8" s="70">
         <v>2</v>
       </c>
-      <c r="W8" s="77" t="s">
+      <c r="W8" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="X8" s="77" t="s">
+      <c r="X8" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="Y8" s="77" t="s">
+      <c r="Y8" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="Z8" s="77" t="s">
+      <c r="Z8" s="70" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:26" ht="15.75">
-      <c r="B9" s="80"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="68"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="79"/>
       <c r="G9" s="12" t="s">
         <v>25</v>
       </c>
@@ -2915,18 +2915,18 @@
       <c r="N9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="77"/>
-      <c r="U9" s="77"/>
-      <c r="V9" s="77"/>
-      <c r="W9" s="77"/>
-      <c r="X9" s="77"/>
-      <c r="Y9" s="77"/>
-      <c r="Z9" s="77"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
+      <c r="Y9" s="70"/>
+      <c r="Z9" s="70"/>
     </row>
     <row r="10" spans="2:26" ht="15.75">
       <c r="B10" s="13" t="s">
@@ -3023,10 +3023,10 @@
       <c r="C12" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="123">
+      <c r="E12" s="42">
         <v>200</v>
       </c>
       <c r="F12" s="15" t="s">
@@ -3175,27 +3175,43 @@
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="64"/>
     </row>
     <row r="25" spans="2:9">
-      <c r="B25" s="47"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="64"/>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B6:B9"/>
@@ -3212,22 +3228,6 @@
     <mergeCell ref="T7:Z7"/>
     <mergeCell ref="G7:N7"/>
     <mergeCell ref="O7:S7"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F7:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3241,8 +3241,8 @@
   </sheetPr>
   <dimension ref="B1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -3262,65 +3262,65 @@
   <sheetData>
     <row r="1" spans="2:14">
       <c r="B1" s="11"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="115" t="s">
+      <c r="D4" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="108" t="s">
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="109"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:14" ht="14.65" thickBot="1">
-      <c r="B5" s="107"/>
-      <c r="C5" s="114"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="110" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="110" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="J5" s="111"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3332,22 +3332,22 @@
       <c r="B6" s="20">
         <v>9</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="94" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="120" t="s">
+      <c r="E6" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="117" t="s">
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="J6" s="118"/>
+      <c r="J6" s="100"/>
       <c r="K6" s="21">
         <v>0</v>
       </c>
@@ -3359,20 +3359,20 @@
       <c r="B7" s="20">
         <v>10</v>
       </c>
-      <c r="C7" s="112"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="86" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="108" t="s">
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="J7" s="109"/>
+      <c r="J7" s="88"/>
       <c r="K7" s="20">
         <v>0</v>
       </c>
@@ -3384,20 +3384,20 @@
       <c r="B8" s="20">
         <v>11</v>
       </c>
-      <c r="C8" s="112"/>
+      <c r="C8" s="94"/>
       <c r="D8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="108" t="s">
+      <c r="E8" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="108" t="s">
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="J8" s="109"/>
+      <c r="J8" s="88"/>
       <c r="K8" s="20">
         <v>200</v>
       </c>
@@ -3425,86 +3425,86 @@
       <c r="K10" s="22"/>
     </row>
     <row r="11" spans="2:14" ht="15" thickTop="1" thickBot="1">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="83" t="s">
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="84"/>
-      <c r="H11" s="81" t="s">
+      <c r="G11" s="104"/>
+      <c r="H11" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="103" t="s">
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="104"/>
+      <c r="N11" s="90"/>
     </row>
     <row r="12" spans="2:14" ht="14.65" thickTop="1">
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="96" t="s">
+      <c r="E12" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="87" t="s">
+      <c r="F12" s="106" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="85" t="s">
+      <c r="G12" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="88" t="s">
+      <c r="H12" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="90" t="s">
+      <c r="I12" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="90" t="s">
+      <c r="J12" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="92" t="s">
+      <c r="K12" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="100" t="s">
+      <c r="L12" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="M12" s="102" t="s">
+      <c r="M12" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="N12" s="86" t="s">
+      <c r="N12" s="95" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="95"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="87"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="106"/>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>3</v>
       </c>
       <c r="C14" s="23">
@@ -3513,8 +3513,10 @@
       <c r="D14" s="23">
         <v>0</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25">
+      <c r="E14" s="122">
+        <v>1</v>
+      </c>
+      <c r="F14" s="24">
         <v>0</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -3523,37 +3525,42 @@
       <c r="H14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>SUM(J14:K14)</f>
         <v>0</v>
       </c>
       <c r="J14" s="23">
         <v>0</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="26">
         <v>0</v>
       </c>
-      <c r="L14" s="28"/>
+      <c r="L14" s="123">
+        <v>1</v>
+      </c>
       <c r="M14" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="27">
         <f>C14</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="C4:C5"/>
@@ -3561,22 +3568,19 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="M11:N11"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="J12:J13"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3590,15 +3594,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D554F47F16D1AE46AF74397CE0A37779" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="24441d7a3758428b2811889d7d94fa0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="28a9ec7f-d5a2-44c1-9222-13672e632811" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c373de015648521c434ab6f3362511f8" ns2:_="">
     <xsd:import namespace="28a9ec7f-d5a2-44c1-9222-13672e632811"/>
@@ -3736,6 +3731,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E90290D4-F465-4AA6-9F9B-036B86358D26}">
   <ds:schemaRefs>
@@ -3746,14 +3750,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E38DC80-6F0A-473F-856D-44FA13F6FA7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24DA1C50-4D4C-432D-94C8-A2B13520658D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3769,4 +3765,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E38DC80-6F0A-473F-856D-44FA13F6FA7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>